<commit_message>
change npoi to openXml
</commit_message>
<xml_diff>
--- a/_template/UserImport.xlsx
+++ b/_template/UserImport.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20415" windowHeight="7785"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20420" windowHeight="7790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -63,12 +63,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -77,8 +92,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -375,31 +393,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -409,7 +434,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -422,7 +447,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>